<commit_message>
Added new Features and new code
</commit_message>
<xml_diff>
--- a/PLANILHA DE PROJETOS E CUSTOS.xlsx
+++ b/PLANILHA DE PROJETOS E CUSTOS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -484,44 +484,122 @@
           <t>FORMA DE PAGTO</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>REGULARIZAÇÕES</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>asdasd</t>
+          <t>popo</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>asdasd</t>
-        </is>
-      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>asdasd</t>
-        </is>
-      </c>
+      <c r="E2" t="inlineStr"/>
       <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>22/12</t>
-        </is>
+      <c r="G2" t="n">
+        <v>23</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>05/08</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>159904</t>
-        </is>
+          <t>25/07</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>20000</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>cartao</t>
+          <t>Pix</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>heloo</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>dontknow</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>25/05/2025</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>500000</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>Dinheiro</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Kenza Asana Rama</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>26/07/2024</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>26/07/2025</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>35000</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Pix</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>nan</t>
         </is>
       </c>
     </row>

</xml_diff>